<commit_message>
added functionality for Extent Report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\DataDrivenGrid\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79FC2DD-6639-4EDC-B09E-937A7784EB02}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800B10CF-13AB-4195-9CCC-F11B2A70E154}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39240" yWindow="3330" windowWidth="20865" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
+    <workbookView xWindow="1380" yWindow="390" windowWidth="20865" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>TestCases</t>
   </si>
@@ -495,7 +495,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78939DD-E20B-419D-B45B-DFA0009D20C1}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -559,55 +559,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -615,121 +580,20 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed bug -removed @beforesuite for setup
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\DataDrivenGrid\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800B10CF-13AB-4195-9CCC-F11B2A70E154}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EEC612-8DFA-45B8-A757-A696B7DEF4A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="390" windowWidth="20865" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>TestCases</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>firstname</t>
@@ -498,7 +495,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D7" sqref="D7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,16 +510,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,16 +527,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -547,16 +544,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,10 +566,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
+      <c r="D7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -580,21 +580,27 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added extent report in context with threading
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\DataDrivenGrid\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EEC612-8DFA-45B8-A757-A696B7DEF4A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C005D09C-956D-49E8-BDD3-00075042B2E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="390" windowWidth="20865" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>TestCases</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>arnav k</t>
+  </si>
+  <si>
+    <t>arnav</t>
   </si>
 </sst>
 </file>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78939DD-E20B-419D-B45B-DFA0009D20C1}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,37 +562,40 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -594,12 +603,40 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>